<commit_message>
[MOSIP-14336] Updating Masterdata Utility
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/upload/xlsx_files/applicant_valid_document.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/upload/xlsx_files/applicant_valid_document.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,1476 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>applicantTypeCode</t>
+          <t>lang_code</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>docCategoryCode</t>
+          <t>apptyp_code</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>docTypeCode</t>
+          <t>doccat_code</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>langCode</t>
+          <t>doctyp_code</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>isActive</t>
+          <t>is_active</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>POI</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>CIN</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>eng</t>
-        </is>
-      </c>
       <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>7</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>7</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>7</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>8</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>8</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>9</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>9</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>9</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>9</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>9</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>10</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>10</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>10</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>10</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>11</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>11</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>11</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>11</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>12</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>12</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>12</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>13</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>13</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>13</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>13</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>13</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>14</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>14</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>14</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>14</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>15</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>15</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>15</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>CRN</t>
+        </is>
+      </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>15</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>16</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>POI</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>16</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>POB</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>16</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>POE</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>COE</t>
+        </is>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>7</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>8</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>11</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>12</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>15</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>POA</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>RNC</t>
+        </is>
+      </c>
+      <c r="E64" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>